<commit_message>
Fixes to setNextPaymentDate and add total to lrc command
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guy/development/pfm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7849F9-4600-6743-8617-AA9F23FD584F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B9253-4E91-7648-B6A8-FDDCE300A918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="4" xr2:uid="{85AD0008-0B75-1E47-AD5E-9735196642DC}"/>
   </bookViews>
@@ -19,6 +19,11 @@
     <sheet name="Account" sheetId="2" r:id="rId4"/>
     <sheet name="Recurring Charge" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="CATEGORY">Category!$B$5:$D$31</definedName>
+    <definedName name="CURRENCY">Currencies!$B$3:$E$170</definedName>
+    <definedName name="PAYEE">Payee!$B$4:$F$22</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="475">
   <si>
     <t>Afghani</t>
   </si>
@@ -1411,14 +1416,69 @@
   </si>
   <si>
     <t>recurring_charge</t>
+  </si>
+  <si>
+    <t>Electricity bill</t>
+  </si>
+  <si>
+    <t>1m</t>
+  </si>
+  <si>
+    <t>Gas bill</t>
+  </si>
+  <si>
+    <t>Water bill</t>
+  </si>
+  <si>
+    <t>Mobile bill</t>
+  </si>
+  <si>
+    <t>Home insurance</t>
+  </si>
+  <si>
+    <t>Car insurance</t>
+  </si>
+  <si>
+    <t>Council tax</t>
+  </si>
+  <si>
+    <t>BT Broadband</t>
+  </si>
+  <si>
+    <t>Mortgage payment</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>Apple Inc</t>
+  </si>
+  <si>
+    <t>AppleCare + (MacBook Pro)</t>
+  </si>
+  <si>
+    <t>1y</t>
+  </si>
+  <si>
+    <t>NSPRO</t>
+  </si>
+  <si>
+    <t>Nesspresso</t>
+  </si>
+  <si>
+    <t>Nesspresso subscription</t>
+  </si>
+  <si>
+    <t>28d</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1482,13 +1542,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1829,7 +1890,7 @@
   <dimension ref="B4:D31"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2160,7 +2221,7 @@
   <dimension ref="B2:F170"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+      <selection activeCell="B3" sqref="B3:E170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4946,10 +5007,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9DDC590-2B98-534C-99BF-725245EB1545}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H38"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4:F22"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4995,15 +5056,15 @@
       </c>
       <c r="E4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -5018,15 +5079,15 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:F21" ca="1" si="0">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H5" t="str">
-        <f t="shared" ref="H5:H22" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-08-02', '2024-08-02');</v>
+        <f t="shared" ref="H5:H24" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -5041,15 +5102,15 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -5064,15 +5125,15 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -5087,15 +5148,15 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -5110,15 +5171,15 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -5133,15 +5194,15 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -5156,15 +5217,15 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -5179,15 +5240,15 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -5202,15 +5263,15 @@
       </c>
       <c r="E13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -5225,15 +5286,15 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -5248,15 +5309,15 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -5271,15 +5332,15 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -5294,15 +5355,15 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -5317,15 +5378,15 @@
       </c>
       <c r="E18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -5340,15 +5401,15 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -5363,15 +5424,15 @@
       </c>
       <c r="E20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H20" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B20 &amp; ", " &amp; CHAR(39) &amp; $C20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="21" spans="2:8">
@@ -5386,15 +5447,15 @@
       </c>
       <c r="E21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -5408,17 +5469,161 @@
         <v>448</v>
       </c>
       <c r="E22" s="5">
-        <f t="shared" ref="E22:F22" ca="1" si="2">TODAY()</f>
-        <v>45506</v>
+        <f t="shared" ref="E22:F24" ca="1" si="2">TODAY()</f>
+        <v>45507</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-08-02', '2024-08-02');</v>
-      </c>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-08-03', '2024-08-03');</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8">
+      <c r="B23" s="4">
+        <v>20</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>468</v>
+      </c>
+      <c r="E23" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45507</v>
+      </c>
+      <c r="F23" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45507</v>
+      </c>
+      <c r="H23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (20, 'APPLE', 'Apple Inc', '2024-08-03', '2024-08-03');</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8">
+      <c r="B24" s="4">
+        <v>21</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>472</v>
+      </c>
+      <c r="E24" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45507</v>
+      </c>
+      <c r="F24" s="5">
+        <f t="shared" ca="1" si="2"/>
+        <v>45507</v>
+      </c>
+      <c r="H24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (21, 'NSPRO', 'Nesspresso', '2024-08-03', '2024-08-03');</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+    </row>
+    <row r="26" spans="2:8">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+    </row>
+    <row r="27" spans="2:8">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+    </row>
+    <row r="28" spans="2:8">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+    </row>
+    <row r="29" spans="2:8">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:8">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+    </row>
+    <row r="31" spans="2:8">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+    </row>
+    <row r="32" spans="2:8">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+    </row>
+    <row r="33" spans="2:6">
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+    </row>
+    <row r="34" spans="2:6">
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+    </row>
+    <row r="35" spans="2:6">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+    </row>
+    <row r="37" spans="2:6">
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5429,7 +5634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4569783B-9638-A94B-85FF-4F96225485BA}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
@@ -5496,15 +5701,15 @@
       </c>
       <c r="H4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="I4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; $E4 &amp; ", " &amp; $F4 &amp; ", " &amp; $G4 &amp; ", " &amp; CHAR(39) &amp; TEXT($H4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -5528,15 +5733,15 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ref="H5:I6" ca="1" si="0">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" ref="K5:K6" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; $E5 &amp; ", " &amp; $F5 &amp; ", " &amp; $G5 &amp; ", " &amp; CHAR(39) &amp; TEXT($H5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="6" spans="2:11">
@@ -5560,15 +5765,15 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-08-02', '2024-08-02');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -5751,7 +5956,7 @@
   <dimension ref="B2:M23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -5804,264 +6009,494 @@
       <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5">
+        <v>45413</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="H4" s="6">
+        <v>127.63</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="M4" t="str">
-        <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; $C4 &amp; ", " &amp; $D4 &amp; ", " &amp; $E4 &amp; ", " &amp; CHAR(39) &amp; $F4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G4 &amp; CHAR(39) &amp; ", " &amp; $H4 &amp; ", " &amp; CHAR(39) &amp; $I4 &amp; CHAR(39) &amp; CHAR(39) &amp; TEXT($J4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (1, , , , '', '', , '''2024-08-02', '2024-08-02');</v>
+        <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; $C4 &amp; ", " &amp; $D4 &amp; ", " &amp; $E4 &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G4 &amp; CHAR(39) &amp; ", " &amp; $H4 &amp; ", " &amp; CHAR(39) &amp; $I4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (1, 1, 2, 1, '2024-05-01', 'Electricity bill', 127.63, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="5" spans="2:13">
       <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>1</v>
+      </c>
+      <c r="F5" s="5">
+        <v>45413</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="H5" s="6">
+        <v>115.86</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:K23" ca="1" si="0">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M5" t="str">
+        <f t="shared" ref="M5:M16" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; $C5 &amp; ", " &amp; $D5 &amp; ", " &amp; $E5 &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G5 &amp; CHAR(39) &amp; ", " &amp; $H5 &amp; ", " &amp; CHAR(39) &amp; $I5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (2, 1, 2, 1, '2024-05-01', 'Gas bill', 115.86, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="6" spans="2:13">
       <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="5">
+        <v>45451</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>460</v>
+      </c>
+      <c r="H6" s="6">
+        <v>85.24</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (3, 1, 2, 5, '2024-06-08', 'Water bill', 85.24, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="7" spans="2:13">
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
+      <c r="C7" s="4">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2</v>
+      </c>
+      <c r="E7" s="4">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5">
+        <v>45427</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="H7" s="6">
+        <v>185.63</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (4, 1, 2, 4, '2024-05-15', 'Mobile bill', 185.63, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="8" spans="2:13">
       <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
+      <c r="C8" s="4">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>19</v>
+      </c>
+      <c r="E8" s="4">
+        <v>10</v>
+      </c>
+      <c r="F8" s="5">
+        <v>45312</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>462</v>
+      </c>
+      <c r="H8" s="6">
+        <v>45.63</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (5, 1, 19, 10, '2024-01-21', 'Home insurance', 45.63, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="9" spans="2:13">
       <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="C9" s="4">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
+        <v>19</v>
+      </c>
+      <c r="E9" s="4">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5">
+        <v>45309</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="H9" s="6">
+        <v>87.63</v>
+      </c>
+      <c r="I9" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (6, 1, 19, 10, '2024-01-18', 'Car insurance', 87.63, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="10" spans="2:13">
       <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
+      <c r="C10" s="4">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="5">
+        <v>45301</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>464</v>
+      </c>
+      <c r="H10" s="6">
+        <v>365.75</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (7, 1, 17, 2, '2024-01-10', 'Council tax', 365.75, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="11" spans="2:13">
       <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
+      <c r="C11" s="4">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>6</v>
+      </c>
+      <c r="F11" s="5">
+        <v>45387</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="H11" s="6">
+        <v>43.72</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (8, 1, 2, 6, '2024-04-05', 'BT Broadband', 43.72, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="12" spans="2:13">
       <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="C12" s="4">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4">
+        <v>8</v>
+      </c>
+      <c r="F12" s="5">
+        <v>45310</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="H12" s="6">
+        <v>9.98</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (9, 1, 17, 8, '2024-01-19', 'Adobe CC', 9.98, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="13" spans="2:13">
       <c r="B13" s="4">
         <v>10</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
+      <c r="C13" s="4">
+        <v>1</v>
+      </c>
+      <c r="D13" s="4">
+        <v>27</v>
+      </c>
+      <c r="E13" s="4">
+        <v>9</v>
+      </c>
+      <c r="F13" s="5">
+        <v>45317</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="H13" s="6">
+        <v>5</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (10, 1, 27, 9, '2024-01-26', 'RNLI', 5, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="14" spans="2:13">
       <c r="B14" s="4">
         <v>11</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
+      <c r="C14" s="4">
+        <v>1</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="5">
+        <v>45292</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>466</v>
+      </c>
+      <c r="H14" s="6">
+        <v>2750</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>458</v>
+      </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (11, 1, 5, 3, '2024-01-01', 'Mortgage payment', 2750, '1m', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="15" spans="2:13">
       <c r="B15" s="4">
         <v>12</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
+      <c r="C15" s="4">
+        <v>1</v>
+      </c>
+      <c r="D15" s="4">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4">
+        <v>20</v>
+      </c>
+      <c r="F15" s="5">
+        <v>45325</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="H15" s="6">
+        <v>99</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>470</v>
+      </c>
       <c r="J15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (12, 1, 19, 20, '2024-02-03', 'AppleCare + (MacBook Pro)', 99, '1y', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="16" spans="2:13">
       <c r="B16" s="4">
         <v>13</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
+      <c r="C16" s="4">
+        <v>1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>17</v>
+      </c>
+      <c r="E16" s="4">
+        <v>21</v>
+      </c>
+      <c r="F16" s="5">
+        <v>45336</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="H16" s="6">
+        <v>20</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>474</v>
+      </c>
       <c r="J16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
+      </c>
+      <c r="M16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (13, 1, 17, 21, '2024-02-14', 'Nesspresso subscription', 20, '28d', '2024-08-03', '2024-08-03');</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -6071,17 +6506,17 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
+      <c r="F17" s="5"/>
       <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
+      <c r="H17" s="6"/>
       <c r="I17" s="4"/>
       <c r="J17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -6091,17 +6526,17 @@
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
+      <c r="F18" s="5"/>
       <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="H18" s="6"/>
       <c r="I18" s="4"/>
       <c r="J18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -6111,17 +6546,17 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
+      <c r="F19" s="5"/>
       <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="H19" s="6"/>
       <c r="I19" s="4"/>
       <c r="J19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -6131,17 +6566,17 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
+      <c r="F20" s="5"/>
       <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
+      <c r="H20" s="6"/>
       <c r="I20" s="4"/>
       <c r="J20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -6151,17 +6586,17 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="F21" s="5"/>
       <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
+      <c r="H21" s="6"/>
       <c r="I21" s="4"/>
       <c r="J21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
     <row r="22" spans="2:11">
@@ -6171,17 +6606,17 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
+      <c r="F22" s="5"/>
       <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="H22" s="6"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5">
-        <f t="shared" ref="J22:K22" ca="1" si="1">TODAY()</f>
-        <v>45506</v>
+        <f t="shared" ref="J22:K22" ca="1" si="2">TODAY()</f>
+        <v>45507</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" ca="1" si="1"/>
-        <v>45506</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>45507</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -6191,17 +6626,17 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
+      <c r="F23" s="5"/>
       <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="4"/>
       <c r="J23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45506</v>
+        <v>45507</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trying to create views
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guy/development/pfm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B5B9253-4E91-7648-B6A8-FDDCE300A918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{79E931FC-C4A8-2240-8A9B-C20B2AA28A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="4" xr2:uid="{85AD0008-0B75-1E47-AD5E-9735196642DC}"/>
   </bookViews>
@@ -25,6 +25,7 @@
     <definedName name="PAYEE">Payee!$B$4:$F$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1477,8 +1478,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="166" formatCode="&quot;£&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3">
     <font>
@@ -1548,8 +1549,8 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5056,15 +5057,15 @@
       </c>
       <c r="E4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="5" spans="2:8">
@@ -5079,15 +5080,15 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:F21" ca="1" si="0">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ref="H5:H24" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="6" spans="2:8">
@@ -5102,15 +5103,15 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="7" spans="2:8">
@@ -5125,15 +5126,15 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="8" spans="2:8">
@@ -5148,15 +5149,15 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="9" spans="2:8">
@@ -5171,15 +5172,15 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="10" spans="2:8">
@@ -5194,15 +5195,15 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="11" spans="2:8">
@@ -5217,15 +5218,15 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="12" spans="2:8">
@@ -5240,15 +5241,15 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="13" spans="2:8">
@@ -5263,15 +5264,15 @@
       </c>
       <c r="E13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="14" spans="2:8">
@@ -5286,15 +5287,15 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="15" spans="2:8">
@@ -5309,15 +5310,15 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="16" spans="2:8">
@@ -5332,15 +5333,15 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="17" spans="2:8">
@@ -5355,15 +5356,15 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="18" spans="2:8">
@@ -5378,15 +5379,15 @@
       </c>
       <c r="E18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="19" spans="2:8">
@@ -5401,15 +5402,15 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="20" spans="2:8">
@@ -5424,15 +5425,15 @@
       </c>
       <c r="E20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H20" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B20 &amp; ", " &amp; CHAR(39) &amp; $C20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="21" spans="2:8">
@@ -5447,15 +5448,15 @@
       </c>
       <c r="E21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="22" spans="2:8">
@@ -5470,15 +5471,15 @@
       </c>
       <c r="E22" s="5">
         <f t="shared" ref="E22:F24" ca="1" si="2">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="23" spans="2:8">
@@ -5493,15 +5494,15 @@
       </c>
       <c r="E23" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (20, 'APPLE', 'Apple Inc', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (20, 'APPLE', 'Apple Inc', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="24" spans="2:8">
@@ -5516,15 +5517,15 @@
       </c>
       <c r="E24" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (21, 'NSPRO', 'Nesspresso', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (21, 'NSPRO', 'Nesspresso', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="25" spans="2:8">
@@ -5700,16 +5701,16 @@
         <v>65</v>
       </c>
       <c r="H4" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <f t="shared" ref="H4:I6" ca="1" si="0">TODAY()</f>
+        <v>45529</v>
       </c>
       <c r="I4" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45529</v>
       </c>
       <c r="K4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; $E4 &amp; ", " &amp; $F4 &amp; ", " &amp; $G4 &amp; ", " &amp; CHAR(39) &amp; TEXT($H4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -5732,16 +5733,16 @@
         <v>65</v>
       </c>
       <c r="H5" s="5">
-        <f t="shared" ref="H5:I6" ca="1" si="0">TODAY()</f>
-        <v>45507</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>45529</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K5" t="str">
-        <f t="shared" ref="K5:K6" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; $E5 &amp; ", " &amp; $F5 &amp; ", " &amp; $G5 &amp; ", " &amp; CHAR(39) &amp; TEXT($H5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-08-03', '2024-08-03');</v>
+        <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; $E5 &amp; ", " &amp; $F5 &amp; ", " &amp; $G5 &amp; ", " &amp; CHAR(39) &amp; TEXT($H5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="6" spans="2:11">
@@ -5765,15 +5766,15 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-08-03', '2024-08-03');</v>
+        <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B6 &amp; ", " &amp; CHAR(39) &amp; $C6 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D6 &amp; CHAR(39) &amp; ", " &amp; $E6 &amp; ", " &amp; $F6 &amp; ", " &amp; $G6 &amp; ", " &amp; CHAR(39) &amp; TEXT($H6, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I6, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -5964,6 +5965,7 @@
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
     <col min="2" max="2" width="4.5" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="3.1640625" customWidth="1"/>
     <col min="13" max="13" width="87.1640625" customWidth="1"/>
   </cols>
@@ -6032,15 +6034,15 @@
       </c>
       <c r="J4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; $C4 &amp; ", " &amp; $D4 &amp; ", " &amp; $E4 &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G4 &amp; CHAR(39) &amp; ", " &amp; $H4 &amp; ", " &amp; CHAR(39) &amp; $I4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (1, 1, 2, 1, '2024-05-01', 'Electricity bill', 127.63, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (1, 1, 2, 1, '2024-05-01', 'Electricity bill', 127.63, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="5" spans="2:13">
@@ -6070,15 +6072,15 @@
       </c>
       <c r="J5" s="5">
         <f t="shared" ref="J5:K23" ca="1" si="0">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M5" t="str">
         <f t="shared" ref="M5:M16" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; $C5 &amp; ", " &amp; $D5 &amp; ", " &amp; $E5 &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G5 &amp; CHAR(39) &amp; ", " &amp; $H5 &amp; ", " &amp; CHAR(39) &amp; $I5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (2, 1, 2, 1, '2024-05-01', 'Gas bill', 115.86, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (2, 1, 2, 1, '2024-05-01', 'Gas bill', 115.86, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="6" spans="2:13">
@@ -6108,15 +6110,15 @@
       </c>
       <c r="J6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (3, 1, 2, 5, '2024-06-08', 'Water bill', 85.24, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (3, 1, 2, 5, '2024-06-08', 'Water bill', 85.24, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="7" spans="2:13">
@@ -6146,15 +6148,15 @@
       </c>
       <c r="J7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (4, 1, 2, 4, '2024-05-15', 'Mobile bill', 185.63, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (4, 1, 2, 4, '2024-05-15', 'Mobile bill', 185.63, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="8" spans="2:13">
@@ -6184,15 +6186,15 @@
       </c>
       <c r="J8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (5, 1, 19, 10, '2024-01-21', 'Home insurance', 45.63, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (5, 1, 19, 10, '2024-01-21', 'Home insurance', 45.63, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="9" spans="2:13">
@@ -6222,15 +6224,15 @@
       </c>
       <c r="J9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (6, 1, 19, 10, '2024-01-18', 'Car insurance', 87.63, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (6, 1, 19, 10, '2024-01-18', 'Car insurance', 87.63, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="10" spans="2:13">
@@ -6260,15 +6262,15 @@
       </c>
       <c r="J10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (7, 1, 17, 2, '2024-01-10', 'Council tax', 365.75, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (7, 1, 17, 2, '2024-01-10', 'Council tax', 365.75, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="11" spans="2:13">
@@ -6298,15 +6300,15 @@
       </c>
       <c r="J11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (8, 1, 2, 6, '2024-04-05', 'BT Broadband', 43.72, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (8, 1, 2, 6, '2024-04-05', 'BT Broadband', 43.72, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="12" spans="2:13">
@@ -6336,15 +6338,15 @@
       </c>
       <c r="J12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (9, 1, 17, 8, '2024-01-19', 'Adobe CC', 9.98, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (9, 1, 17, 8, '2024-01-19', 'Adobe CC', 9.98, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="13" spans="2:13">
@@ -6374,15 +6376,15 @@
       </c>
       <c r="J13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (10, 1, 27, 9, '2024-01-26', 'RNLI', 5, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (10, 1, 27, 9, '2024-01-26', 'RNLI', 5, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="14" spans="2:13">
@@ -6412,15 +6414,15 @@
       </c>
       <c r="J14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (11, 1, 5, 3, '2024-01-01', 'Mortgage payment', 2750, '1m', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (11, 1, 5, 3, '2024-01-01', 'Mortgage payment', 2750, '1m', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="15" spans="2:13">
@@ -6450,15 +6452,15 @@
       </c>
       <c r="J15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (12, 1, 19, 20, '2024-02-03', 'AppleCare + (MacBook Pro)', 99, '1y', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (12, 1, 19, 20, '2024-02-03', 'AppleCare + (MacBook Pro)', 99, '1y', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="16" spans="2:13">
@@ -6488,15 +6490,15 @@
       </c>
       <c r="J16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="M16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (13, 1, 17, 21, '2024-02-14', 'Nesspresso subscription', 20, '28d', '2024-08-03', '2024-08-03');</v>
+        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (13, 1, 17, 21, '2024-02-14', 'Nesspresso subscription', 20, '28d', '2024-08-25', '2024-08-25');</v>
       </c>
     </row>
     <row r="17" spans="2:11">
@@ -6512,11 +6514,11 @@
       <c r="I17" s="4"/>
       <c r="J17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="18" spans="2:11">
@@ -6532,11 +6534,11 @@
       <c r="I18" s="4"/>
       <c r="J18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="19" spans="2:11">
@@ -6552,11 +6554,11 @@
       <c r="I19" s="4"/>
       <c r="J19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="20" spans="2:11">
@@ -6572,11 +6574,11 @@
       <c r="I20" s="4"/>
       <c r="J20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="21" spans="2:11">
@@ -6592,11 +6594,11 @@
       <c r="I21" s="4"/>
       <c r="J21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
     <row r="22" spans="2:11">
@@ -6611,12 +6613,12 @@
       <c r="H22" s="6"/>
       <c r="I22" s="4"/>
       <c r="J22" s="5">
-        <f t="shared" ref="J22:K22" ca="1" si="2">TODAY()</f>
-        <v>45507</v>
+        <f ca="1">TODAY()</f>
+        <v>45529</v>
       </c>
       <c r="K22" s="5">
-        <f t="shared" ca="1" si="2"/>
-        <v>45507</v>
+        <f ca="1">TODAY()</f>
+        <v>45529</v>
       </c>
     </row>
     <row r="23" spans="2:11">
@@ -6632,11 +6634,11 @@
       <c r="I23" s="4"/>
       <c r="J23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
       <c r="K23" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45507</v>
+        <v>45529</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add import function for budgets
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/guy/development/pfm/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2A4CD4-6C9F-AD43-A3E3-A66C557FD93D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A62B31F-ED63-5C4D-993C-77235F805961}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="3" xr2:uid="{85AD0008-0B75-1E47-AD5E-9735196642DC}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="22500" activeTab="4" xr2:uid="{85AD0008-0B75-1E47-AD5E-9735196642DC}"/>
   </bookViews>
   <sheets>
     <sheet name="Category" sheetId="4" r:id="rId1"/>
@@ -25,7 +25,6 @@
     <definedName name="PAYEE">Payee!$B$4:$F$22</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -46,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="477">
   <si>
     <t>Afghani</t>
   </si>
@@ -1398,15 +1397,6 @@
     <t>Sainsburys</t>
   </si>
   <si>
-    <t>account_id</t>
-  </si>
-  <si>
-    <t>category_id</t>
-  </si>
-  <si>
-    <t>payee_id</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -1416,9 +1406,6 @@
     <t>frequency</t>
   </si>
   <si>
-    <t>recurring_charge</t>
-  </si>
-  <si>
     <t>Electricity bill</t>
   </si>
   <si>
@@ -1471,6 +1458,24 @@
   </si>
   <si>
     <t>28d</t>
+  </si>
+  <si>
+    <t>endDate</t>
+  </si>
+  <si>
+    <t>accountCode</t>
+  </si>
+  <si>
+    <t>categoryCode</t>
+  </si>
+  <si>
+    <t>payeeCode</t>
+  </si>
+  <si>
+    <t>DBRecurringCharge</t>
+  </si>
+  <si>
+    <t>MTGE</t>
   </si>
 </sst>
 </file>
@@ -5057,15 +5062,15 @@
       </c>
       <c r="E4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F4" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (1, 'EDF', 'EDF Energy', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J4" t="str">
         <f>"{" &amp; CHAR(34) &amp; $C4 &amp; CHAR(34) &amp; "," &amp; CHAR(34) &amp;  $D4 &amp; CHAR(34) &amp; "},"</f>
@@ -5084,15 +5089,15 @@
       </c>
       <c r="E5" s="5">
         <f t="shared" ref="E5:F21" ca="1" si="0">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H5" t="str">
         <f t="shared" ref="H5:H24" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (2, 'BEXL', 'Bexley Borough Council', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J5" t="str">
         <f t="shared" ref="J5:J24" si="2">"{" &amp; CHAR(34) &amp; $C5 &amp; CHAR(34) &amp; "," &amp; CHAR(34) &amp;  $D5 &amp; CHAR(34) &amp; "},"</f>
@@ -5111,15 +5116,15 @@
       </c>
       <c r="E6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (3, 'HALFX', 'Halifax Building Society', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
@@ -5138,15 +5143,15 @@
       </c>
       <c r="E7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H7" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (4, 'VODA', 'Vodafone', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J7" t="str">
         <f t="shared" si="2"/>
@@ -5165,15 +5170,15 @@
       </c>
       <c r="E8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H8" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (5, 'TWAT', 'Thames Water', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J8" t="str">
         <f t="shared" si="2"/>
@@ -5192,15 +5197,15 @@
       </c>
       <c r="E9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H9" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (6, 'BT', 'British Telecommunications', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J9" t="str">
         <f t="shared" si="2"/>
@@ -5219,15 +5224,15 @@
       </c>
       <c r="E10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (7, 'MBNA', 'MBNA Credit Card', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
@@ -5246,15 +5251,15 @@
       </c>
       <c r="E11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (8, 'ADOBE', 'Adobe CC', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
@@ -5273,15 +5278,15 @@
       </c>
       <c r="E12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F12" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (9, 'RNLI', 'RNLI', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
@@ -5300,15 +5305,15 @@
       </c>
       <c r="E13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F13" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (10, 'AVIVA', 'Aviva Insurance', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
@@ -5327,15 +5332,15 @@
       </c>
       <c r="E14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (11, 'SAINS', 'Sainsburys', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
@@ -5354,15 +5359,15 @@
       </c>
       <c r="E15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (12, 'ASDA', 'Asda Supermarket', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
@@ -5381,15 +5386,15 @@
       </c>
       <c r="E16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (13, 'TFL', 'Transport for London', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
@@ -5408,15 +5413,15 @@
       </c>
       <c r="E17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (14, 'WASAB', 'Wasabi Bento', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
@@ -5435,15 +5440,15 @@
       </c>
       <c r="E18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (15, 'PRET', 'Pret a Manger', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
@@ -5462,15 +5467,15 @@
       </c>
       <c r="E19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F19" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (16, 'UBER', 'Uber', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="2"/>
@@ -5489,15 +5494,15 @@
       </c>
       <c r="E20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F20" s="5">
         <f ca="1">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H20" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ") VALUES (" &amp; $B20 &amp; ", " &amp; CHAR(39) &amp; $C20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D20 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($E20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($F20, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (17, 'AMAZN', 'Amazon', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="2"/>
@@ -5516,15 +5521,15 @@
       </c>
       <c r="E21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (18, 'MAS', 'Marks &amp; Spencer', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="2"/>
@@ -5543,15 +5548,15 @@
       </c>
       <c r="E22" s="5">
         <f t="shared" ref="E22:F24" ca="1" si="3">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (19, 'BAQ', 'B &amp; Q', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
@@ -5563,22 +5568,22 @@
         <v>20</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="E23" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (20, 'APPLE', 'Apple Inc', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (20, 'APPLE', 'Apple Inc', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
@@ -5590,22 +5595,22 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="E24" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (21, 'NSPRO', 'Nesspresso', '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO payee (id, code, name, created, updated) VALUES (21, 'NSPRO', 'Nesspresso', '2024-09-21', '2024-09-21');</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
@@ -5720,7 +5725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4569783B-9638-A94B-85FF-4F96225485BA}">
   <dimension ref="B2:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K4" sqref="K4:K6"/>
     </sheetView>
   </sheetViews>
@@ -5787,15 +5792,15 @@
       </c>
       <c r="H4" s="5">
         <f t="shared" ref="H4:I6" ca="1" si="0">TODAY()</f>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="I4" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="K4" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; CHAR(39) &amp; $C4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D4 &amp; CHAR(39) &amp; ", " &amp; $E4 &amp; ", " &amp; $F4 &amp; ", " &amp; $G4 &amp; ", " &amp; CHAR(39) &amp; TEXT($H4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (1, 'HSBC Current Account', 'HSBC', 1280.28, 1280.28, 65, '2024-09-21', '2024-09-21');</v>
       </c>
     </row>
     <row r="5" spans="2:11">
@@ -5819,15 +5824,15 @@
       </c>
       <c r="H5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="I5" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="K5" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; CHAR(39) &amp; $C5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D5 &amp; CHAR(39) &amp; ", " &amp; $E5 &amp; ", " &amp; $F5 &amp; ", " &amp; $G5 &amp; ", " &amp; CHAR(39) &amp; TEXT($H5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (2, 'Lloyds ISA', 'LISA', 8192.67, 8192.67, 65, '2024-09-21', '2024-09-21');</v>
       </c>
     </row>
     <row r="6" spans="2:11">
@@ -5851,15 +5856,15 @@
       </c>
       <c r="H6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="I6" s="5">
         <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
+        <v>45556</v>
       </c>
       <c r="K6" t="str">
         <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ") VALUES (" &amp; $B6 &amp; ", " &amp; CHAR(39) &amp; $C6 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $D6 &amp; CHAR(39) &amp; ", " &amp; $E6 &amp; ", " &amp; $F6 &amp; ", " &amp; $G6 &amp; ", " &amp; CHAR(39) &amp; TEXT($H6, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($I6, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-09-03', '2024-09-03');</v>
+        <v>INSERT INTO account (id, name, code, opening_balance, current_balance, currency_id, created, updated) VALUES (3, 'MBNA Credit Card', 'MBNA', -2048.94, -2048.94, 65, '2024-09-21', '2024-09-21');</v>
       </c>
     </row>
     <row r="7" spans="2:11">
@@ -6039,379 +6044,260 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88107C30-A2E2-E44B-A8C8-5FC8490E8F04}">
-  <dimension ref="B2:M23"/>
+  <dimension ref="B2:I23"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4:M16"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="3.33203125" customWidth="1"/>
-    <col min="2" max="2" width="4.5" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.6640625" customWidth="1"/>
-    <col min="10" max="10" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="3.1640625" customWidth="1"/>
-    <col min="13" max="13" width="87.1640625" customWidth="1"/>
+    <col min="10" max="10" width="3.1640625" customWidth="1"/>
+    <col min="11" max="11" width="87.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13">
+    <row r="2" spans="2:9">
       <c r="B2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="3" spans="2:13">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9">
       <c r="B3" s="3" t="s">
-        <v>357</v>
+        <v>472</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>451</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>452</v>
-      </c>
       <c r="F3" s="3" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>388</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="4" spans="2:13">
-      <c r="B4" s="4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E4" s="5">
         <v>45413</v>
       </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="4" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="H4" s="6">
         <v>127.63</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J4" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="K4" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="M4" t="str">
-        <f ca="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B4 &amp; ", " &amp; $C4 &amp; ", " &amp; $D4 &amp; ", " &amp; $E4 &amp; ", " &amp; CHAR(39) &amp; TEXT($F4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G4 &amp; CHAR(39) &amp; ", " &amp; $H4 &amp; ", " &amp; CHAR(39) &amp; $I4 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K4, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (1, 1, 2, 1, '2024-05-01', 'Electricity bill', 127.63, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="5" spans="2:13">
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E5" s="5">
         <v>45413</v>
       </c>
+      <c r="F5" s="5"/>
       <c r="G5" s="4" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H5" s="6">
         <v>115.86</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J5" s="5">
-        <f t="shared" ref="J5:K23" ca="1" si="0">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="K5" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M5" t="str">
-        <f t="shared" ref="M5:M16" ca="1" si="1">"INSERT INTO " &amp; $B$2 &amp; " (" &amp; $B$3 &amp; ", " &amp; $C$3 &amp; ", " &amp; $D$3 &amp; ", " &amp; $E$3 &amp; ", " &amp; $F$3 &amp; ", " &amp; $G$3 &amp; ", " &amp; $H$3 &amp; ", " &amp; $I$3 &amp; ", " &amp; $J$3 &amp; ", " &amp; $K$3 &amp; ") VALUES (" &amp; $B5 &amp; ", " &amp; $C5 &amp; ", " &amp; $D5 &amp; ", " &amp; $E5 &amp; ", " &amp; CHAR(39) &amp; TEXT($F5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; $G5 &amp; CHAR(39) &amp; ", " &amp; $H5 &amp; ", " &amp; CHAR(39) &amp; $I5 &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($J5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ", " &amp; CHAR(39) &amp; TEXT($K5, "yyyy-mm-dd") &amp; CHAR(39) &amp; ");"</f>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (2, 1, 2, 1, '2024-05-01', 'Gas bill', 115.86, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="6" spans="2:13">
-      <c r="B6" s="4">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <v>1</v>
-      </c>
-      <c r="D6" s="4">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
-        <v>5</v>
-      </c>
-      <c r="F6" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="E6" s="5">
         <v>45451</v>
       </c>
+      <c r="F6" s="5"/>
       <c r="G6" s="4" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="H6" s="6">
         <v>85.24</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K6" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M6" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (3, 1, 2, 5, '2024-06-08', 'Water bill', 85.24, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="7" spans="2:13">
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
-        <v>4</v>
-      </c>
-      <c r="F7" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>366</v>
+      </c>
+      <c r="E7" s="5">
         <v>45427</v>
       </c>
+      <c r="F7" s="5"/>
       <c r="G7" s="4" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="H7" s="6">
         <v>185.63</v>
       </c>
       <c r="I7" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E8" s="5">
+        <v>45312</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="4" t="s">
         <v>458</v>
-      </c>
-      <c r="J7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K7" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M7" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (4, 1, 2, 4, '2024-05-15', 'Mobile bill', 185.63, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="8" spans="2:13">
-      <c r="B8" s="4">
-        <v>5</v>
-      </c>
-      <c r="C8" s="4">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4">
-        <v>19</v>
-      </c>
-      <c r="E8" s="4">
-        <v>10</v>
-      </c>
-      <c r="F8" s="5">
-        <v>45312</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>462</v>
       </c>
       <c r="H8" s="6">
         <v>45.63</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J8" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K8" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M8" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (5, 1, 19, 10, '2024-01-21', 'Home insurance', 45.63, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="9" spans="2:13">
-      <c r="B9" s="4">
-        <v>6</v>
-      </c>
-      <c r="C9" s="4">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4">
-        <v>19</v>
-      </c>
-      <c r="E9" s="4">
-        <v>10</v>
-      </c>
-      <c r="F9" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="E9" s="5">
         <v>45309</v>
       </c>
+      <c r="F9" s="5"/>
       <c r="G9" s="4" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="H9" s="6">
         <v>87.63</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J9" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K9" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M9" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (6, 1, 19, 10, '2024-01-18', 'Car insurance', 87.63, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="10" spans="2:13">
-      <c r="B10" s="4">
-        <v>7</v>
-      </c>
-      <c r="C10" s="4">
-        <v>1</v>
-      </c>
-      <c r="D10" s="4">
-        <v>17</v>
-      </c>
-      <c r="E10" s="4">
-        <v>2</v>
-      </c>
-      <c r="F10" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>362</v>
+      </c>
+      <c r="E10" s="5">
         <v>45301</v>
       </c>
+      <c r="F10" s="5"/>
       <c r="G10" s="4" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="H10" s="6">
         <v>365.75</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J10" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K10" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M10" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (7, 1, 17, 2, '2024-01-10', 'Council tax', 365.75, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="11" spans="2:13">
-      <c r="B11" s="4">
-        <v>8</v>
-      </c>
-      <c r="C11" s="4">
-        <v>1</v>
-      </c>
-      <c r="D11" s="4">
-        <v>2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>6</v>
-      </c>
-      <c r="F11" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>370</v>
+      </c>
+      <c r="E11" s="5">
         <v>45387</v>
       </c>
+      <c r="F11" s="5"/>
       <c r="G11" s="4" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="H11" s="6">
         <v>43.72</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J11" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K11" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M11" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (8, 1, 2, 6, '2024-04-05', 'BT Broadband', 43.72, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="12" spans="2:13">
-      <c r="B12" s="4">
-        <v>9</v>
-      </c>
-      <c r="C12" s="4">
-        <v>1</v>
-      </c>
-      <c r="D12" s="4">
-        <v>17</v>
-      </c>
-      <c r="E12" s="4">
-        <v>8</v>
-      </c>
-      <c r="F12" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>372</v>
+      </c>
+      <c r="E12" s="5">
         <v>45310</v>
       </c>
+      <c r="F12" s="5"/>
       <c r="G12" s="4" t="s">
         <v>373</v>
       </c>
@@ -6419,37 +6305,23 @@
         <v>9.98</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J12" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K12" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M12" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (9, 1, 17, 8, '2024-01-19', 'Adobe CC', 9.98, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="13" spans="2:13">
-      <c r="B13" s="4">
-        <v>10</v>
-      </c>
-      <c r="C13" s="4">
-        <v>1</v>
-      </c>
-      <c r="D13" s="4">
-        <v>27</v>
-      </c>
-      <c r="E13" s="4">
-        <v>9</v>
-      </c>
-      <c r="F13" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="E13" s="5">
         <v>45317</v>
       </c>
+      <c r="F13" s="5"/>
       <c r="G13" s="4" t="s">
         <v>374</v>
       </c>
@@ -6457,274 +6329,150 @@
         <v>5</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J13" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="K13" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="M13" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (10, 1, 27, 9, '2024-01-26', 'RNLI', 5, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="14" spans="2:13">
-      <c r="B14" s="4">
-        <v>11</v>
-      </c>
-      <c r="C14" s="4">
-        <v>1</v>
-      </c>
-      <c r="D14" s="4">
-        <v>5</v>
-      </c>
-      <c r="E14" s="4">
-        <v>3</v>
-      </c>
-      <c r="F14" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>476</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>364</v>
+      </c>
+      <c r="E14" s="5">
         <v>45292</v>
       </c>
+      <c r="F14" s="5"/>
       <c r="G14" s="4" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="H14" s="6">
         <v>2750</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>458</v>
-      </c>
-      <c r="J14" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K14" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M14" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (11, 1, 5, 3, '2024-01-01', 'Mortgage payment', 2750, '1m', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="15" spans="2:13">
-      <c r="B15" s="4">
-        <v>12</v>
-      </c>
-      <c r="C15" s="4">
-        <v>1</v>
-      </c>
-      <c r="D15" s="4">
-        <v>19</v>
-      </c>
-      <c r="E15" s="4">
-        <v>20</v>
-      </c>
-      <c r="F15" s="5">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="E15" s="5">
         <v>45325</v>
       </c>
+      <c r="F15" s="5"/>
       <c r="G15" s="4" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H15" s="6">
         <v>99</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>470</v>
-      </c>
-      <c r="J15" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K15" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M15" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (12, 1, 19, 20, '2024-02-03', 'AppleCare + (MacBook Pro)', 99, '1y', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="16" spans="2:13">
-      <c r="B16" s="4">
-        <v>13</v>
-      </c>
-      <c r="C16" s="4">
-        <v>1</v>
-      </c>
-      <c r="D16" s="4">
-        <v>17</v>
-      </c>
-      <c r="E16" s="4">
-        <v>21</v>
-      </c>
-      <c r="F16" s="5">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="E16" s="5">
         <v>45336</v>
       </c>
+      <c r="F16" s="5"/>
       <c r="G16" s="4" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="H16" s="6">
         <v>20</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>474</v>
-      </c>
-      <c r="J16" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K16" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="M16" t="str">
-        <f t="shared" ca="1" si="1"/>
-        <v>INSERT INTO recurring_charge (id, account_id, category_id, payee_id, date, description, amount, frequency, created, updated) VALUES (13, 1, 17, 21, '2024-02-14', 'Nesspresso subscription', 20, '28d', '2024-09-03', '2024-09-03');</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11">
-      <c r="B17" s="4">
-        <v>14</v>
-      </c>
+        <v>470</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
       <c r="H17" s="6"/>
       <c r="I17" s="4"/>
-      <c r="J17" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K17" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="18" spans="2:11">
-      <c r="B18" s="4">
-        <v>15</v>
-      </c>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="5"/>
       <c r="F18" s="5"/>
       <c r="G18" s="4"/>
       <c r="H18" s="6"/>
       <c r="I18" s="4"/>
-      <c r="J18" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K18" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="19" spans="2:11">
-      <c r="B19" s="4">
-        <v>16</v>
-      </c>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="4"/>
       <c r="H19" s="6"/>
       <c r="I19" s="4"/>
-      <c r="J19" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K19" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="20" spans="2:11">
-      <c r="B20" s="4">
-        <v>17</v>
-      </c>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="5"/>
       <c r="G20" s="4"/>
       <c r="H20" s="6"/>
       <c r="I20" s="4"/>
-      <c r="J20" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="K20" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="21" spans="2:11">
-      <c r="B21" s="4">
-        <v>18</v>
-      </c>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
+      <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="4"/>
       <c r="H21" s="6"/>
       <c r="I21" s="4"/>
-      <c r="J21" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K21" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11">
-      <c r="B22" s="4">
-        <v>19</v>
-      </c>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
+      <c r="E22" s="5"/>
       <c r="F22" s="5"/>
       <c r="G22" s="4"/>
       <c r="H22" s="6"/>
       <c r="I22" s="4"/>
-      <c r="J22" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-      <c r="K22" s="5">
-        <f ca="1">TODAY()</f>
-        <v>45538</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11">
-      <c r="B23" s="4">
-        <v>20</v>
-      </c>
+    </row>
+    <row r="23" spans="2:9">
+      <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
+      <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="4"/>
       <c r="H23" s="6"/>
       <c r="I23" s="4"/>
-      <c r="J23" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
-      <c r="K23" s="5">
-        <f t="shared" ca="1" si="0"/>
-        <v>45538</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>